<commit_message>
feat: add tests and lucas doc
</commit_message>
<xml_diff>
--- a/docs/assets/Avaliacao_Heuristica.xlsx
+++ b/docs/assets/Avaliacao_Heuristica.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="87">
   <si>
     <t>PARECER TÉCNICO: AVALIAÇÃO HEURÍSTICA</t>
   </si>
@@ -172,6 +172,63 @@
     <t>Botões de ajuda em lugares chaves poderiam ajudar sem gerar a necessidade de criar todo um tutorial.</t>
   </si>
   <si>
+    <t>sem problemas</t>
+  </si>
+  <si>
+    <t>Dificuldade em entender diferenças entre registrar alimento/refeição</t>
+  </si>
+  <si>
+    <t>procurar deixar mais claro a diferença enttre cada um, avaliando elementos na UI</t>
+  </si>
+  <si>
+    <t>As opções de deletar não requerem double-check</t>
+  </si>
+  <si>
+    <t>avaliar opções crticas e requerir confirmação</t>
+  </si>
+  <si>
+    <t>Houve uma leve demora para entender que o botão de criar o alimento aparecia apos pesquisar por ele e não existir</t>
+  </si>
+  <si>
+    <t>avaliar se há como deixar ainda mais facil a opção de criar alimento</t>
+  </si>
+  <si>
+    <t>Houve problemas na eficacia do registro de alimentações bem como dos valores consumidos</t>
+  </si>
+  <si>
+    <t>criar valores padrão para serem adicionados/registrados e ddiminuir cliques para registrar refeições.</t>
+  </si>
+  <si>
+    <t>Houve dificuldade para entender a parte de registro do plano de alimentação. Não há uma documentação clara sobre o uso do sistema.</t>
+  </si>
+  <si>
+    <t>Documentar uso do sistema ou fornecer tutoriais.</t>
+  </si>
+  <si>
+    <t>O usuário esperava um botão "Cadastrar Novo Alimento" fora do fluxo de registro.</t>
+  </si>
+  <si>
+    <t>Entra de acordo com o botão criar que aparece quando se pesquisa um alimento que ainda não existe.</t>
+  </si>
+  <si>
+    <t>Demorou para perceber que o botão "Criar" aparece após a pesquisa não ser encontrada</t>
+  </si>
+  <si>
+    <t>AAvaliar forma mais explicita para criação de alimentos</t>
+  </si>
+  <si>
+    <t>O usuário demorou para achar a aba Receita dentro do modal de registro. Não percebeu a distinção visual entre as abas "Alimento" e "Receita" imediatamente.</t>
+  </si>
+  <si>
+    <t>Deixar mais explicita a diferença entre o cadastro de alimento e receita visualmente</t>
+  </si>
+  <si>
+    <t>Falta de um guia ou tutorial rápido/onboarding para as funcionalidades menos óbvias indica que o sistema não é completamente utilizável sem alguma forma de documentação ou auxílio.</t>
+  </si>
+  <si>
+    <t>Criar tutorial ou documentação de uso</t>
+  </si>
+  <si>
     <t>Existiu certa confusão nas terminologias (refeição, alimento, receita)</t>
   </si>
   <si>
@@ -317,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -385,6 +442,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -13389,7 +13449,9 @@
       <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="E6" s="11"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -13423,8 +13485,12 @@
       <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -13457,7 +13523,9 @@
       <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="11"/>
+      <c r="D8" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="E8" s="11"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -13491,7 +13559,9 @@
       <c r="C9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="E9" s="11"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -13525,8 +13595,12 @@
       <c r="C10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
@@ -13559,8 +13633,12 @@
       <c r="C11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+      <c r="D11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -13593,8 +13671,12 @@
       <c r="C12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
@@ -13627,7 +13709,9 @@
       <c r="C13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="E13" s="22"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -13661,7 +13745,9 @@
       <c r="C14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="E14" s="14"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -13695,8 +13781,12 @@
       <c r="C15" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -19660,7 +19750,9 @@
       <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="E6" s="11"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -19694,7 +19786,9 @@
       <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="E7" s="11"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -19728,8 +19822,12 @@
       <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
@@ -19762,7 +19860,9 @@
       <c r="C9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="E9" s="11"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -19796,7 +19896,9 @@
       <c r="C10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="E10" s="11"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -19830,8 +19932,12 @@
       <c r="C11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+      <c r="D11" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>65</v>
+      </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -19864,7 +19970,9 @@
       <c r="C12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="E12" s="11"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -19898,8 +20006,12 @@
       <c r="C13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
+      <c r="D13" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>67</v>
+      </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -19932,7 +20044,9 @@
       <c r="C14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="E14" s="14"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -19966,8 +20080,12 @@
       <c r="C15" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>69</v>
+      </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -25968,10 +26086,10 @@
         <v>14</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -26042,10 +26160,10 @@
         <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -26152,7 +26270,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="13"/>
@@ -26260,10 +26378,10 @@
         <v>39</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -32229,7 +32347,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="13"/>
@@ -32265,10 +32383,10 @@
         <v>14</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -32303,7 +32421,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="13"/>
@@ -32339,10 +32457,10 @@
         <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -32377,7 +32495,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="13"/>
@@ -32413,10 +32531,10 @@
         <v>25</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -32451,7 +32569,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="13"/>
@@ -32487,7 +32605,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="13"/>
@@ -32523,7 +32641,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="13"/>
@@ -32557,10 +32675,10 @@
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="12" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -32588,7 +32706,7 @@
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="24"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>

</xml_diff>